<commit_message>
1) Adding the LTSpice model for the new PPS330D 2) Updating shunt resistor in the ReferenceGuide.xlsx to show the actual resistor specified in the BOM
</commit_message>
<xml_diff>
--- a/Hardware/LAB-ASDM300F/docs/ReferenceGuide.xlsx
+++ b/Hardware/LAB-ASDM300F/docs/ReferenceGuide.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="13920" windowHeight="8505" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="13920" windowHeight="8505" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Coincident Domains" sheetId="1" r:id="rId1"/>
@@ -1088,8 +1088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1137,20 +1137,19 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D10" si="0">B2*C2</f>
+        <f t="shared" ref="D2:D3" si="0">B2*C2</f>
         <v>300</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E8" si="1">3.3/(100*D2/1000)</f>
+        <f t="shared" ref="E2:E3" si="1">3.3/(100*D2/1000)</f>
         <v>0.11</v>
       </c>
       <c r="F2">
-        <f>E2</f>
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="G2">
         <f>1000*(3.3/4096)/(F2/10)</f>
-        <v>73.2421875</v>
+        <v>80.56640625</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1172,12 +1171,11 @@
         <v>0.11</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3" si="2">E3</f>
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G17" si="3">1000*(3.3/4096)/(F3/10)</f>
-        <v>73.2421875</v>
+        <f t="shared" ref="G3" si="2">1000*(3.3/4096)/(F3/10)</f>
+        <v>80.56640625</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1471,7 +1469,7 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <f>F$6*(G8*(1/G$6+1/H$6)-H8/H$6)+G8</f>
+        <f t="shared" ref="F8:F41" si="1">F$6*(G8*(1/G$6+1/H$6)-H8/H$6)+G8</f>
         <v>3.3214285714285716</v>
       </c>
       <c r="G8">
@@ -1481,7 +1479,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="10">
-        <f>A8-A9</f>
+        <f t="shared" ref="J8:J40" si="2">A8-A9</f>
         <v>5.8928571428571441E-2</v>
       </c>
       <c r="K8" s="10">
@@ -1489,7 +1487,7 @@
         <v>5.9090909090909083E-2</v>
       </c>
       <c r="N8">
-        <f>A8-F8</f>
+        <f t="shared" ref="N8:N41" si="3">A8-F8</f>
         <v>4.6777003484320456E-2</v>
       </c>
       <c r="P8" s="6"/>
@@ -1512,7 +1510,7 @@
         <v>0.1</v>
       </c>
       <c r="F9">
-        <f>F$6*(G9*(1/G$6+1/H$6)-H9/H$6)+G9</f>
+        <f t="shared" si="1"/>
         <v>3.2623376623376625</v>
       </c>
       <c r="G9">
@@ -1522,15 +1520,15 @@
         <v>0.1</v>
       </c>
       <c r="J9" s="10">
-        <f>A9-A10</f>
+        <f t="shared" si="2"/>
         <v>5.8928571428570997E-2</v>
       </c>
       <c r="K9" s="10">
-        <f t="shared" ref="K9:K40" si="1">F9-F10</f>
+        <f t="shared" ref="K9:K40" si="4">F9-F10</f>
         <v>5.9090909090909083E-2</v>
       </c>
       <c r="N9">
-        <f>A9-F9</f>
+        <f t="shared" si="3"/>
         <v>4.6939341146658098E-2</v>
       </c>
       <c r="P9" s="6"/>
@@ -1538,7 +1536,7 @@
         <v>62000</v>
       </c>
       <c r="U9">
-        <f>T9/J8</f>
+        <f t="shared" ref="U9:U34" si="5">T9/J8</f>
         <v>1052121.2121212119</v>
       </c>
     </row>
@@ -1554,7 +1552,7 @@
         <v>0.2</v>
       </c>
       <c r="F10">
-        <f>F$6*(G10*(1/G$6+1/H$6)-H10/H$6)+G10</f>
+        <f t="shared" si="1"/>
         <v>3.2032467532467535</v>
       </c>
       <c r="G10">
@@ -1564,15 +1562,15 @@
         <v>0.2</v>
       </c>
       <c r="J10" s="10">
-        <f>A10-A11</f>
+        <f t="shared" si="2"/>
         <v>5.8928571428571441E-2</v>
       </c>
       <c r="K10" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5.9090909090909083E-2</v>
       </c>
       <c r="N10">
-        <f>A10-F10</f>
+        <f t="shared" si="3"/>
         <v>4.7101678808996184E-2</v>
       </c>
       <c r="P10" s="6"/>
@@ -1580,7 +1578,7 @@
         <v>68000</v>
       </c>
       <c r="U10">
-        <f>T10/J9</f>
+        <f t="shared" si="5"/>
         <v>1153939.3939394024</v>
       </c>
     </row>
@@ -1596,7 +1594,7 @@
         <v>0.3</v>
       </c>
       <c r="F11">
-        <f>F$6*(G11*(1/G$6+1/H$6)-H11/H$6)+G11</f>
+        <f t="shared" si="1"/>
         <v>3.1441558441558444</v>
       </c>
       <c r="G11">
@@ -1606,15 +1604,15 @@
         <v>0.3</v>
       </c>
       <c r="J11" s="10">
-        <f>A11-A12</f>
+        <f t="shared" si="2"/>
         <v>5.8928571428571885E-2</v>
       </c>
       <c r="K11" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5.9090909090909527E-2</v>
       </c>
       <c r="N11">
-        <f>A11-F11</f>
+        <f t="shared" si="3"/>
         <v>4.7264016471333825E-2</v>
       </c>
       <c r="P11" s="6"/>
@@ -1622,7 +1620,7 @@
         <v>75000</v>
       </c>
       <c r="U11">
-        <f>T11/J10</f>
+        <f t="shared" si="5"/>
         <v>1272727.2727272725</v>
       </c>
     </row>
@@ -1638,7 +1636,7 @@
         <v>0.4</v>
       </c>
       <c r="F12">
-        <f>F$6*(G12*(1/G$6+1/H$6)-H12/H$6)+G12</f>
+        <f t="shared" si="1"/>
         <v>3.0850649350649348</v>
       </c>
       <c r="G12">
@@ -1648,15 +1646,15 @@
         <v>0.4</v>
       </c>
       <c r="J12" s="10">
-        <f>A12-A13</f>
+        <f t="shared" si="2"/>
         <v>5.8928571428571441E-2</v>
       </c>
       <c r="K12" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5.9090909090908639E-2</v>
       </c>
       <c r="N12">
-        <f>A12-F12</f>
+        <f t="shared" si="3"/>
         <v>4.7426354133671467E-2</v>
       </c>
       <c r="P12" s="6"/>
@@ -1664,7 +1662,7 @@
         <v>82000</v>
       </c>
       <c r="U12">
-        <f>T12/J11</f>
+        <f t="shared" si="5"/>
         <v>1391515.1515151407</v>
       </c>
     </row>
@@ -1680,7 +1678,7 @@
         <v>0.5</v>
       </c>
       <c r="F13">
-        <f>F$6*(G13*(1/G$6+1/H$6)-H13/H$6)+G13</f>
+        <f t="shared" si="1"/>
         <v>3.0259740259740262</v>
       </c>
       <c r="G13">
@@ -1690,15 +1688,15 @@
         <v>0.5</v>
       </c>
       <c r="J13" s="10">
-        <f>A13-A14</f>
+        <f t="shared" si="2"/>
         <v>5.8928571428571441E-2</v>
       </c>
       <c r="K13" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5.9090909090909527E-2</v>
       </c>
       <c r="N13">
-        <f>A13-F13</f>
+        <f t="shared" si="3"/>
         <v>4.7588691796008664E-2</v>
       </c>
       <c r="P13" s="6"/>
@@ -1706,7 +1704,7 @@
         <v>91000</v>
       </c>
       <c r="U13">
-        <f>T13/J12</f>
+        <f t="shared" si="5"/>
         <v>1544242.4242424238</v>
       </c>
     </row>
@@ -1722,7 +1720,7 @@
         <v>0.6</v>
       </c>
       <c r="F14">
-        <f>F$6*(G14*(1/G$6+1/H$6)-H14/H$6)+G14</f>
+        <f t="shared" si="1"/>
         <v>2.9668831168831167</v>
       </c>
       <c r="G14">
@@ -1732,15 +1730,15 @@
         <v>0.6</v>
       </c>
       <c r="J14" s="10">
-        <f>A14-A15</f>
+        <f t="shared" si="2"/>
         <v>5.8928571428571441E-2</v>
       </c>
       <c r="K14" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5.9090909090908639E-2</v>
       </c>
       <c r="N14">
-        <f>A14-F14</f>
+        <f t="shared" si="3"/>
         <v>4.775102945834675E-2</v>
       </c>
       <c r="P14" s="7"/>
@@ -1748,7 +1746,7 @@
         <v>100000</v>
       </c>
       <c r="U14">
-        <f>T14/J13</f>
+        <f t="shared" si="5"/>
         <v>1696969.6969696966</v>
       </c>
     </row>
@@ -1764,7 +1762,7 @@
         <v>0.7</v>
       </c>
       <c r="F15">
-        <f>F$6*(G15*(1/G$6+1/H$6)-H15/H$6)+G15</f>
+        <f t="shared" si="1"/>
         <v>2.907792207792208</v>
       </c>
       <c r="G15">
@@ -1774,15 +1772,15 @@
         <v>0.7</v>
       </c>
       <c r="J15" s="10">
-        <f>A15-A16</f>
+        <f t="shared" si="2"/>
         <v>5.8928571428570997E-2</v>
       </c>
       <c r="K15" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5.9090909090909083E-2</v>
       </c>
       <c r="N15">
-        <f>A15-F15</f>
+        <f t="shared" si="3"/>
         <v>4.7913367120683947E-2</v>
       </c>
       <c r="P15" s="6"/>
@@ -1790,7 +1788,7 @@
         <v>110000</v>
       </c>
       <c r="U15">
-        <f>T15/J14</f>
+        <f t="shared" si="5"/>
         <v>1866666.6666666663</v>
       </c>
     </row>
@@ -1803,30 +1801,30 @@
         <v>0.6</v>
       </c>
       <c r="C16">
-        <f t="shared" ref="C16:C22" si="2">C15+0.1</f>
+        <f t="shared" ref="C16:C22" si="6">C15+0.1</f>
         <v>0.79999999999999993</v>
       </c>
       <c r="F16">
-        <f>F$6*(G16*(1/G$6+1/H$6)-H16/H$6)+G16</f>
+        <f t="shared" si="1"/>
         <v>2.848701298701299</v>
       </c>
       <c r="G16">
         <v>1.1000000000000001</v>
       </c>
       <c r="H16">
-        <f t="shared" ref="H16:H22" si="3">H15+0.1</f>
+        <f t="shared" ref="H16:H22" si="7">H15+0.1</f>
         <v>0.79999999999999993</v>
       </c>
       <c r="J16" s="10">
-        <f>A16-A17</f>
+        <f t="shared" si="2"/>
         <v>5.8928571428571441E-2</v>
       </c>
       <c r="K16" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5.9090909090909083E-2</v>
       </c>
       <c r="N16">
-        <f>A16-F16</f>
+        <f t="shared" si="3"/>
         <v>4.8075704783022033E-2</v>
       </c>
       <c r="P16" s="6"/>
@@ -1834,7 +1832,7 @@
         <v>120000</v>
       </c>
       <c r="U16">
-        <f>T16/J15</f>
+        <f t="shared" si="5"/>
         <v>2036363.6363636514</v>
       </c>
     </row>
@@ -1847,30 +1845,30 @@
         <v>0.6</v>
       </c>
       <c r="C17">
+        <f t="shared" si="6"/>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>2.7896103896103899</v>
+      </c>
+      <c r="G17">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="7"/>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="J17" s="10">
         <f t="shared" si="2"/>
-        <v>0.89999999999999991</v>
-      </c>
-      <c r="F17">
-        <f>F$6*(G17*(1/G$6+1/H$6)-H17/H$6)+G17</f>
-        <v>2.7896103896103899</v>
-      </c>
-      <c r="G17">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H17">
+        <v>5.8928571428571885E-2</v>
+      </c>
+      <c r="K17" s="10">
+        <f t="shared" si="4"/>
+        <v>5.9090909090909083E-2</v>
+      </c>
+      <c r="N17">
         <f t="shared" si="3"/>
-        <v>0.89999999999999991</v>
-      </c>
-      <c r="J17" s="10">
-        <f>A17-A18</f>
-        <v>5.8928571428571885E-2</v>
-      </c>
-      <c r="K17" s="10">
-        <f t="shared" si="1"/>
-        <v>5.9090909090909083E-2</v>
-      </c>
-      <c r="N17">
-        <f>A17-F17</f>
         <v>4.8238042445359675E-2</v>
       </c>
       <c r="P17" s="6"/>
@@ -1878,7 +1876,7 @@
         <v>130000</v>
       </c>
       <c r="U17">
-        <f>T17/J16</f>
+        <f t="shared" si="5"/>
         <v>2206060.6060606055</v>
       </c>
       <c r="Y17" s="6"/>
@@ -1892,30 +1890,30 @@
         <v>0.6</v>
       </c>
       <c r="C18">
+        <f t="shared" si="6"/>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="F18" s="5">
+        <f t="shared" si="1"/>
+        <v>2.7305194805194808</v>
+      </c>
+      <c r="G18" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H18" s="5">
+        <f t="shared" si="7"/>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="J18" s="10">
         <f t="shared" si="2"/>
-        <v>0.99999999999999989</v>
-      </c>
-      <c r="F18" s="5">
-        <f>F$6*(G18*(1/G$6+1/H$6)-H18/H$6)+G18</f>
-        <v>2.7305194805194808</v>
-      </c>
-      <c r="G18" s="5">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H18" s="5">
+        <v>5.8928571428570997E-2</v>
+      </c>
+      <c r="K18" s="10">
+        <f t="shared" si="4"/>
+        <v>5.9090909090909083E-2</v>
+      </c>
+      <c r="N18">
         <f t="shared" si="3"/>
-        <v>0.99999999999999989</v>
-      </c>
-      <c r="J18" s="10">
-        <f>A18-A19</f>
-        <v>5.8928571428570997E-2</v>
-      </c>
-      <c r="K18" s="10">
-        <f t="shared" si="1"/>
-        <v>5.9090909090909083E-2</v>
-      </c>
-      <c r="N18">
-        <f>A18-F18</f>
         <v>4.8400380107696872E-2</v>
       </c>
       <c r="P18" s="6"/>
@@ -1923,7 +1921,7 @@
         <v>150000</v>
       </c>
       <c r="U18">
-        <f>T18/J17</f>
+        <f t="shared" si="5"/>
         <v>2545454.5454545259</v>
       </c>
       <c r="V18" s="5"/>
@@ -1937,30 +1935,30 @@
         <v>0.6</v>
       </c>
       <c r="C19">
+        <f t="shared" si="6"/>
+        <v>1.0999999999999999</v>
+      </c>
+      <c r="F19" s="5">
+        <f t="shared" si="1"/>
+        <v>2.6714285714285717</v>
+      </c>
+      <c r="G19" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H19" s="5">
+        <f t="shared" si="7"/>
+        <v>1.0999999999999999</v>
+      </c>
+      <c r="J19" s="10">
         <f t="shared" si="2"/>
-        <v>1.0999999999999999</v>
-      </c>
-      <c r="F19" s="5">
-        <f>F$6*(G19*(1/G$6+1/H$6)-H19/H$6)+G19</f>
-        <v>2.6714285714285717</v>
-      </c>
-      <c r="G19" s="5">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H19" s="5">
+        <v>5.8928571428571885E-2</v>
+      </c>
+      <c r="K19" s="10">
+        <f t="shared" si="4"/>
+        <v>5.9090909090909527E-2</v>
+      </c>
+      <c r="N19">
         <f t="shared" si="3"/>
-        <v>1.0999999999999999</v>
-      </c>
-      <c r="J19" s="10">
-        <f>A19-A20</f>
-        <v>5.8928571428571885E-2</v>
-      </c>
-      <c r="K19" s="10">
-        <f t="shared" si="1"/>
-        <v>5.9090909090909527E-2</v>
-      </c>
-      <c r="N19">
-        <f>A19-F19</f>
         <v>4.8562717770034958E-2</v>
       </c>
       <c r="P19" s="6"/>
@@ -1968,7 +1966,7 @@
         <v>160000</v>
       </c>
       <c r="U19">
-        <f>T19/J18</f>
+        <f t="shared" si="5"/>
         <v>2715151.5151515352</v>
       </c>
       <c r="V19" s="4"/>
@@ -1982,30 +1980,30 @@
         <v>0.6</v>
       </c>
       <c r="C20">
+        <f t="shared" si="6"/>
+        <v>1.2</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>2.6123376623376622</v>
+      </c>
+      <c r="G20">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="7"/>
+        <v>1.2</v>
+      </c>
+      <c r="J20" s="10">
         <f t="shared" si="2"/>
-        <v>1.2</v>
-      </c>
-      <c r="F20">
-        <f>F$6*(G20*(1/G$6+1/H$6)-H20/H$6)+G20</f>
-        <v>2.6123376623376622</v>
-      </c>
-      <c r="G20">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H20">
+        <v>5.8928571428571441E-2</v>
+      </c>
+      <c r="K20" s="10">
+        <f t="shared" si="4"/>
+        <v>5.9090909090908639E-2</v>
+      </c>
+      <c r="N20">
         <f t="shared" si="3"/>
-        <v>1.2</v>
-      </c>
-      <c r="J20" s="10">
-        <f>A20-A21</f>
-        <v>5.8928571428571441E-2</v>
-      </c>
-      <c r="K20" s="10">
-        <f t="shared" si="1"/>
-        <v>5.9090909090908639E-2</v>
-      </c>
-      <c r="N20">
-        <f>A20-F20</f>
         <v>4.8725055432372599E-2</v>
       </c>
       <c r="P20" s="6"/>
@@ -2013,7 +2011,7 @@
         <v>180000</v>
       </c>
       <c r="U20">
-        <f>T20/J19</f>
+        <f t="shared" si="5"/>
         <v>3054545.4545454308</v>
       </c>
     </row>
@@ -2026,30 +2024,30 @@
         <v>0.6</v>
       </c>
       <c r="C21">
+        <f t="shared" si="6"/>
+        <v>1.3</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>2.5532467532467535</v>
+      </c>
+      <c r="G21">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="7"/>
+        <v>1.3</v>
+      </c>
+      <c r="J21" s="10">
         <f t="shared" si="2"/>
-        <v>1.3</v>
-      </c>
-      <c r="F21">
-        <f>F$6*(G21*(1/G$6+1/H$6)-H21/H$6)+G21</f>
-        <v>2.5532467532467535</v>
-      </c>
-      <c r="G21">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H21">
+        <v>5.8928571428571441E-2</v>
+      </c>
+      <c r="K21" s="10">
+        <f t="shared" si="4"/>
+        <v>5.9090909090909527E-2</v>
+      </c>
+      <c r="N21">
         <f t="shared" si="3"/>
-        <v>1.3</v>
-      </c>
-      <c r="J21" s="10">
-        <f>A21-A22</f>
-        <v>5.8928571428571441E-2</v>
-      </c>
-      <c r="K21" s="10">
-        <f t="shared" si="1"/>
-        <v>5.9090909090909527E-2</v>
-      </c>
-      <c r="N21">
-        <f>A21-F21</f>
         <v>4.8887393094709797E-2</v>
       </c>
       <c r="P21" s="6"/>
@@ -2057,7 +2055,7 @@
         <v>200000</v>
       </c>
       <c r="U21">
-        <f>T21/J20</f>
+        <f t="shared" si="5"/>
         <v>3393939.3939393931</v>
       </c>
     </row>
@@ -2070,30 +2068,30 @@
         <v>0.6</v>
       </c>
       <c r="C22">
+        <f t="shared" si="6"/>
+        <v>1.4000000000000001</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>2.494155844155844</v>
+      </c>
+      <c r="G22">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="7"/>
+        <v>1.4000000000000001</v>
+      </c>
+      <c r="J22" s="10">
         <f t="shared" si="2"/>
-        <v>1.4000000000000001</v>
-      </c>
-      <c r="F22">
-        <f>F$6*(G22*(1/G$6+1/H$6)-H22/H$6)+G22</f>
-        <v>2.494155844155844</v>
-      </c>
-      <c r="G22">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H22">
+        <v>5.8928571428571441E-2</v>
+      </c>
+      <c r="K22" s="10">
+        <f t="shared" si="4"/>
+        <v>5.9090909090908639E-2</v>
+      </c>
+      <c r="N22">
         <f t="shared" si="3"/>
-        <v>1.4000000000000001</v>
-      </c>
-      <c r="J22" s="10">
-        <f>A22-A23</f>
-        <v>5.8928571428571441E-2</v>
-      </c>
-      <c r="K22" s="10">
-        <f t="shared" si="1"/>
-        <v>5.9090909090908639E-2</v>
-      </c>
-      <c r="N22">
-        <f>A22-F22</f>
         <v>4.9049730757047882E-2</v>
       </c>
       <c r="P22" s="6"/>
@@ -2101,7 +2099,7 @@
         <v>220000</v>
       </c>
       <c r="U22">
-        <f>T22/J21</f>
+        <f t="shared" si="5"/>
         <v>3733333.3333333326</v>
       </c>
     </row>
@@ -2118,7 +2116,7 @@
         <v>1.5000000000000002</v>
       </c>
       <c r="F23">
-        <f>F$6*(G23*(1/G$6+1/H$6)-H23/H$6)+G23</f>
+        <f t="shared" si="1"/>
         <v>2.4350649350649354</v>
       </c>
       <c r="G23">
@@ -2129,15 +2127,15 @@
         <v>1.5000000000000002</v>
       </c>
       <c r="J23" s="10">
-        <f>A23-A24</f>
+        <f t="shared" si="2"/>
         <v>5.8928571428571441E-2</v>
       </c>
       <c r="K23" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5.9090909090909527E-2</v>
       </c>
       <c r="N23">
-        <f>A23-F23</f>
+        <f t="shared" si="3"/>
         <v>4.921206841938508E-2</v>
       </c>
       <c r="P23" s="6"/>
@@ -2145,7 +2143,7 @@
         <v>240000</v>
       </c>
       <c r="U23">
-        <f>T23/J22</f>
+        <f t="shared" si="5"/>
         <v>4072727.272727272</v>
       </c>
     </row>
@@ -2162,7 +2160,7 @@
         <v>1.6000000000000003</v>
       </c>
       <c r="F24">
-        <f>F$6*(G24*(1/G$6+1/H$6)-H24/H$6)+G24</f>
+        <f t="shared" si="1"/>
         <v>2.3759740259740258</v>
       </c>
       <c r="G24">
@@ -2173,15 +2171,15 @@
         <v>1.6000000000000003</v>
       </c>
       <c r="J24" s="10">
-        <f>A24-A25</f>
+        <f t="shared" si="2"/>
         <v>5.8928571428571441E-2</v>
       </c>
       <c r="K24" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5.9090909090909083E-2</v>
       </c>
       <c r="N24">
-        <f>A24-F24</f>
+        <f t="shared" si="3"/>
         <v>4.9374406081723166E-2</v>
       </c>
       <c r="P24" s="6"/>
@@ -2189,7 +2187,7 @@
         <v>270000</v>
       </c>
       <c r="U24">
-        <f>T24/J23</f>
+        <f t="shared" si="5"/>
         <v>4581818.1818181807</v>
       </c>
     </row>
@@ -2206,7 +2204,7 @@
         <v>1.7000000000000004</v>
       </c>
       <c r="F25">
-        <f>F$6*(G25*(1/G$6+1/H$6)-H25/H$6)+G25</f>
+        <f t="shared" si="1"/>
         <v>2.3168831168831168</v>
       </c>
       <c r="G25">
@@ -2217,15 +2215,15 @@
         <v>1.7000000000000004</v>
       </c>
       <c r="J25" s="10">
-        <f>A25-A26</f>
+        <f t="shared" si="2"/>
         <v>5.8928571428571441E-2</v>
       </c>
       <c r="K25" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5.9090909090909083E-2</v>
       </c>
       <c r="N25">
-        <f>A25-F25</f>
+        <f t="shared" si="3"/>
         <v>4.9536743744060807E-2</v>
       </c>
       <c r="P25" s="6"/>
@@ -2233,7 +2231,7 @@
         <v>300000</v>
       </c>
       <c r="U25">
-        <f>T25/J24</f>
+        <f t="shared" si="5"/>
         <v>5090909.0909090899</v>
       </c>
     </row>
@@ -2250,7 +2248,7 @@
         <v>1.8000000000000005</v>
       </c>
       <c r="F26">
-        <f>F$6*(G26*(1/G$6+1/H$6)-H26/H$6)+G26</f>
+        <f t="shared" si="1"/>
         <v>2.2577922077922077</v>
       </c>
       <c r="G26">
@@ -2261,15 +2259,15 @@
         <v>1.8000000000000005</v>
       </c>
       <c r="J26" s="10">
-        <f>A26-A27</f>
+        <f t="shared" si="2"/>
         <v>5.8928571428571441E-2</v>
       </c>
       <c r="K26" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5.9090909090909083E-2</v>
       </c>
       <c r="N26">
-        <f>A26-F26</f>
+        <f t="shared" si="3"/>
         <v>4.9699081406398449E-2</v>
       </c>
       <c r="P26" s="6"/>
@@ -2277,7 +2275,7 @@
         <v>330000</v>
       </c>
       <c r="U26">
-        <f>T26/J25</f>
+        <f t="shared" si="5"/>
         <v>5599999.9999999991</v>
       </c>
     </row>
@@ -2290,30 +2288,30 @@
         <v>0.6</v>
       </c>
       <c r="C27">
-        <f t="shared" ref="C27:C38" si="4">C26+0.1</f>
+        <f t="shared" ref="C27:C38" si="8">C26+0.1</f>
         <v>1.9000000000000006</v>
       </c>
       <c r="F27">
-        <f>F$6*(G27*(1/G$6+1/H$6)-H27/H$6)+G27</f>
+        <f t="shared" si="1"/>
         <v>2.1987012987012986</v>
       </c>
       <c r="G27">
         <v>1.1000000000000001</v>
       </c>
       <c r="H27">
-        <f t="shared" ref="H27:H41" si="5">H26+0.1</f>
+        <f t="shared" ref="H27:H41" si="9">H26+0.1</f>
         <v>1.9000000000000006</v>
       </c>
       <c r="J27" s="10">
-        <f>A27-A28</f>
+        <f t="shared" si="2"/>
         <v>5.8928571428571441E-2</v>
       </c>
       <c r="K27" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5.9090909090909083E-2</v>
       </c>
       <c r="N27">
-        <f>A27-F27</f>
+        <f t="shared" si="3"/>
         <v>4.986141906873609E-2</v>
       </c>
       <c r="P27" s="6"/>
@@ -2321,7 +2319,7 @@
         <v>360000</v>
       </c>
       <c r="U27">
-        <f>T27/J26</f>
+        <f t="shared" si="5"/>
         <v>6109090.9090909073</v>
       </c>
     </row>
@@ -2334,30 +2332,30 @@
         <v>0.6</v>
       </c>
       <c r="C28">
+        <f t="shared" si="8"/>
+        <v>2.0000000000000004</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>2.1396103896103895</v>
+      </c>
+      <c r="G28">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="9"/>
+        <v>2.0000000000000004</v>
+      </c>
+      <c r="J28" s="10">
+        <f t="shared" si="2"/>
+        <v>5.8928571428571885E-2</v>
+      </c>
+      <c r="K28" s="10">
         <f t="shared" si="4"/>
-        <v>2.0000000000000004</v>
-      </c>
-      <c r="F28">
-        <f>F$6*(G28*(1/G$6+1/H$6)-H28/H$6)+G28</f>
-        <v>2.1396103896103895</v>
-      </c>
-      <c r="G28">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H28">
-        <f t="shared" si="5"/>
-        <v>2.0000000000000004</v>
-      </c>
-      <c r="J28" s="10">
-        <f>A28-A29</f>
-        <v>5.8928571428571885E-2</v>
-      </c>
-      <c r="K28" s="10">
-        <f t="shared" si="1"/>
         <v>5.9090909090909527E-2</v>
       </c>
       <c r="N28">
-        <f>A28-F28</f>
+        <f t="shared" si="3"/>
         <v>5.0023756731073732E-2</v>
       </c>
       <c r="P28" s="6"/>
@@ -2365,7 +2363,7 @@
         <v>390000</v>
       </c>
       <c r="U28">
-        <f>T28/J27</f>
+        <f t="shared" si="5"/>
         <v>6618181.8181818165</v>
       </c>
     </row>
@@ -2378,30 +2376,30 @@
         <v>0.6</v>
       </c>
       <c r="C29">
+        <f t="shared" si="8"/>
+        <v>2.1000000000000005</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="1"/>
+        <v>2.08051948051948</v>
+      </c>
+      <c r="G29">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="9"/>
+        <v>2.1000000000000005</v>
+      </c>
+      <c r="J29" s="10">
+        <f t="shared" si="2"/>
+        <v>5.8928571428570997E-2</v>
+      </c>
+      <c r="K29" s="10">
         <f t="shared" si="4"/>
-        <v>2.1000000000000005</v>
-      </c>
-      <c r="F29">
-        <f>F$6*(G29*(1/G$6+1/H$6)-H29/H$6)+G29</f>
-        <v>2.08051948051948</v>
-      </c>
-      <c r="G29">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H29">
-        <f t="shared" si="5"/>
-        <v>2.1000000000000005</v>
-      </c>
-      <c r="J29" s="10">
-        <f>A29-A30</f>
-        <v>5.8928571428570997E-2</v>
-      </c>
-      <c r="K29" s="10">
-        <f t="shared" si="1"/>
         <v>5.9090909090908639E-2</v>
       </c>
       <c r="N29">
-        <f>A29-F29</f>
+        <f t="shared" si="3"/>
         <v>5.0186094393411373E-2</v>
       </c>
       <c r="P29" s="6"/>
@@ -2409,7 +2407,7 @@
         <v>430000</v>
       </c>
       <c r="U29">
-        <f>T29/J28</f>
+        <f t="shared" si="5"/>
         <v>7296969.6969696404</v>
       </c>
     </row>
@@ -2422,30 +2420,30 @@
         <v>0.6</v>
       </c>
       <c r="C30">
+        <f t="shared" si="8"/>
+        <v>2.2000000000000006</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="1"/>
+        <v>2.0214285714285714</v>
+      </c>
+      <c r="G30">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="9"/>
+        <v>2.2000000000000006</v>
+      </c>
+      <c r="J30" s="10">
+        <f t="shared" si="2"/>
+        <v>5.8928571428571441E-2</v>
+      </c>
+      <c r="K30" s="10">
         <f t="shared" si="4"/>
-        <v>2.2000000000000006</v>
-      </c>
-      <c r="F30">
-        <f>F$6*(G30*(1/G$6+1/H$6)-H30/H$6)+G30</f>
-        <v>2.0214285714285714</v>
-      </c>
-      <c r="G30">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H30">
-        <f t="shared" si="5"/>
-        <v>2.2000000000000006</v>
-      </c>
-      <c r="J30" s="10">
-        <f>A30-A31</f>
-        <v>5.8928571428571441E-2</v>
-      </c>
-      <c r="K30" s="10">
-        <f t="shared" si="1"/>
         <v>5.9090909090909305E-2</v>
       </c>
       <c r="N30">
-        <f>A30-F30</f>
+        <f t="shared" si="3"/>
         <v>5.0348432055749015E-2</v>
       </c>
       <c r="P30" s="6"/>
@@ -2453,7 +2451,7 @@
         <v>470000</v>
       </c>
       <c r="U30">
-        <f>T30/J29</f>
+        <f t="shared" si="5"/>
         <v>7975757.5757576339</v>
       </c>
     </row>
@@ -2466,30 +2464,30 @@
         <v>0.6</v>
       </c>
       <c r="C31">
+        <f t="shared" si="8"/>
+        <v>2.3000000000000007</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="1"/>
+        <v>1.962337662337662</v>
+      </c>
+      <c r="G31">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="9"/>
+        <v>2.3000000000000007</v>
+      </c>
+      <c r="J31" s="10">
+        <f t="shared" si="2"/>
+        <v>5.8928571428571441E-2</v>
+      </c>
+      <c r="K31" s="10">
         <f t="shared" si="4"/>
-        <v>2.3000000000000007</v>
-      </c>
-      <c r="F31">
-        <f>F$6*(G31*(1/G$6+1/H$6)-H31/H$6)+G31</f>
-        <v>1.962337662337662</v>
-      </c>
-      <c r="G31">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H31">
-        <f t="shared" si="5"/>
-        <v>2.3000000000000007</v>
-      </c>
-      <c r="J31" s="10">
-        <f>A31-A32</f>
-        <v>5.8928571428571441E-2</v>
-      </c>
-      <c r="K31" s="10">
-        <f t="shared" si="1"/>
         <v>5.9090909090909083E-2</v>
       </c>
       <c r="N31">
-        <f>A31-F31</f>
+        <f t="shared" si="3"/>
         <v>5.0510769718086879E-2</v>
       </c>
       <c r="P31" s="6"/>
@@ -2497,7 +2495,7 @@
         <v>510000</v>
       </c>
       <c r="U31">
-        <f>T31/J30</f>
+        <f t="shared" si="5"/>
         <v>8654545.4545454532</v>
       </c>
     </row>
@@ -2510,30 +2508,30 @@
         <v>0.6</v>
       </c>
       <c r="C32">
+        <f t="shared" si="8"/>
+        <v>2.4000000000000008</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="1"/>
+        <v>1.903246753246753</v>
+      </c>
+      <c r="G32">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="9"/>
+        <v>2.4000000000000008</v>
+      </c>
+      <c r="J32" s="10">
+        <f t="shared" si="2"/>
+        <v>5.8928571428571441E-2</v>
+      </c>
+      <c r="K32" s="10">
         <f t="shared" si="4"/>
-        <v>2.4000000000000008</v>
-      </c>
-      <c r="F32">
-        <f>F$6*(G32*(1/G$6+1/H$6)-H32/H$6)+G32</f>
-        <v>1.903246753246753</v>
-      </c>
-      <c r="G32">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H32">
-        <f t="shared" si="5"/>
-        <v>2.4000000000000008</v>
-      </c>
-      <c r="J32" s="10">
-        <f>A32-A33</f>
-        <v>5.8928571428571441E-2</v>
-      </c>
-      <c r="K32" s="10">
-        <f t="shared" si="1"/>
         <v>5.9090909090909305E-2</v>
       </c>
       <c r="N32">
-        <f>A32-F32</f>
+        <f t="shared" si="3"/>
         <v>5.067310738042452E-2</v>
       </c>
       <c r="P32" s="6"/>
@@ -2541,7 +2539,7 @@
         <v>560000</v>
       </c>
       <c r="U32">
-        <f>T32/J31</f>
+        <f t="shared" si="5"/>
         <v>9503030.3030303009</v>
       </c>
     </row>
@@ -2554,30 +2552,30 @@
         <v>0.6</v>
       </c>
       <c r="C33">
+        <f t="shared" si="8"/>
+        <v>2.5000000000000009</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="1"/>
+        <v>1.8441558441558437</v>
+      </c>
+      <c r="G33">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="9"/>
+        <v>2.5000000000000009</v>
+      </c>
+      <c r="J33" s="10">
+        <f t="shared" si="2"/>
+        <v>5.8928571428571885E-2</v>
+      </c>
+      <c r="K33" s="10">
         <f t="shared" si="4"/>
-        <v>2.5000000000000009</v>
-      </c>
-      <c r="F33">
-        <f>F$6*(G33*(1/G$6+1/H$6)-H33/H$6)+G33</f>
-        <v>1.8441558441558437</v>
-      </c>
-      <c r="G33">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H33">
-        <f t="shared" si="5"/>
-        <v>2.5000000000000009</v>
-      </c>
-      <c r="J33" s="10">
-        <f>A33-A34</f>
-        <v>5.8928571428571885E-2</v>
-      </c>
-      <c r="K33" s="10">
-        <f t="shared" si="1"/>
         <v>5.9090909090909083E-2</v>
       </c>
       <c r="N33">
-        <f>A33-F33</f>
+        <f t="shared" si="3"/>
         <v>5.0835445042762384E-2</v>
       </c>
       <c r="P33" s="6"/>
@@ -2585,7 +2583,7 @@
         <v>620000</v>
       </c>
       <c r="U33">
-        <f>T33/J32</f>
+        <f t="shared" si="5"/>
         <v>10521212.121212119</v>
       </c>
     </row>
@@ -2598,30 +2596,30 @@
         <v>0.6</v>
       </c>
       <c r="C34">
+        <f t="shared" si="8"/>
+        <v>2.600000000000001</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="1"/>
+        <v>1.7850649350649346</v>
+      </c>
+      <c r="G34">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="9"/>
+        <v>2.600000000000001</v>
+      </c>
+      <c r="J34" s="10">
+        <f t="shared" si="2"/>
+        <v>5.8928571428570997E-2</v>
+      </c>
+      <c r="K34" s="10">
         <f t="shared" si="4"/>
-        <v>2.600000000000001</v>
-      </c>
-      <c r="F34">
-        <f>F$6*(G34*(1/G$6+1/H$6)-H34/H$6)+G34</f>
-        <v>1.7850649350649346</v>
-      </c>
-      <c r="G34">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H34">
-        <f t="shared" si="5"/>
-        <v>2.600000000000001</v>
-      </c>
-      <c r="J34" s="10">
-        <f>A34-A35</f>
-        <v>5.8928571428570997E-2</v>
-      </c>
-      <c r="K34" s="10">
-        <f t="shared" si="1"/>
         <v>5.9090909090909083E-2</v>
       </c>
       <c r="N34">
-        <f>A34-F34</f>
+        <f t="shared" si="3"/>
         <v>5.0997782705099581E-2</v>
       </c>
       <c r="P34" s="6"/>
@@ -2629,7 +2627,7 @@
         <v>680000</v>
       </c>
       <c r="U34">
-        <f>T34/J33</f>
+        <f t="shared" si="5"/>
         <v>11539393.93939385</v>
       </c>
     </row>
@@ -2642,30 +2640,30 @@
         <v>0.6</v>
       </c>
       <c r="C35">
+        <f t="shared" si="8"/>
+        <v>2.7000000000000011</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="1"/>
+        <v>1.7259740259740255</v>
+      </c>
+      <c r="G35">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="9"/>
+        <v>2.7000000000000011</v>
+      </c>
+      <c r="J35" s="10">
+        <f t="shared" si="2"/>
+        <v>5.8928571428571885E-2</v>
+      </c>
+      <c r="K35" s="10">
         <f t="shared" si="4"/>
-        <v>2.7000000000000011</v>
-      </c>
-      <c r="F35">
-        <f>F$6*(G35*(1/G$6+1/H$6)-H35/H$6)+G35</f>
-        <v>1.7259740259740255</v>
-      </c>
-      <c r="G35">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H35">
-        <f t="shared" si="5"/>
-        <v>2.7000000000000011</v>
-      </c>
-      <c r="J35" s="10">
-        <f>A35-A36</f>
-        <v>5.8928571428571885E-2</v>
-      </c>
-      <c r="K35" s="10">
-        <f t="shared" si="1"/>
         <v>5.9090909090909083E-2</v>
       </c>
       <c r="N35">
-        <f>A35-F35</f>
+        <f t="shared" si="3"/>
         <v>5.1160120367437667E-2</v>
       </c>
       <c r="P35" s="6"/>
@@ -2679,30 +2677,30 @@
         <v>0.6</v>
       </c>
       <c r="C36">
+        <f t="shared" si="8"/>
+        <v>2.8000000000000012</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="1"/>
+        <v>1.6668831168831164</v>
+      </c>
+      <c r="G36">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="9"/>
+        <v>2.8000000000000012</v>
+      </c>
+      <c r="J36" s="10">
+        <f t="shared" si="2"/>
+        <v>5.8928571428571441E-2</v>
+      </c>
+      <c r="K36" s="10">
         <f t="shared" si="4"/>
-        <v>2.8000000000000012</v>
-      </c>
-      <c r="F36">
-        <f>F$6*(G36*(1/G$6+1/H$6)-H36/H$6)+G36</f>
-        <v>1.6668831168831164</v>
-      </c>
-      <c r="G36">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H36">
-        <f t="shared" si="5"/>
-        <v>2.8000000000000012</v>
-      </c>
-      <c r="J36" s="10">
-        <f>A36-A37</f>
-        <v>5.8928571428571441E-2</v>
-      </c>
-      <c r="K36" s="10">
-        <f t="shared" si="1"/>
         <v>5.9090909090909083E-2</v>
       </c>
       <c r="N36">
-        <f>A36-F36</f>
+        <f t="shared" si="3"/>
         <v>5.1322458029774864E-2</v>
       </c>
       <c r="P36" s="6"/>
@@ -2716,30 +2714,30 @@
         <v>0.6</v>
       </c>
       <c r="C37">
+        <f t="shared" si="8"/>
+        <v>2.9000000000000012</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="1"/>
+        <v>1.6077922077922073</v>
+      </c>
+      <c r="G37">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="9"/>
+        <v>2.9000000000000012</v>
+      </c>
+      <c r="J37" s="10">
+        <f t="shared" si="2"/>
+        <v>5.8928571428571441E-2</v>
+      </c>
+      <c r="K37" s="10">
         <f t="shared" si="4"/>
-        <v>2.9000000000000012</v>
-      </c>
-      <c r="F37">
-        <f>F$6*(G37*(1/G$6+1/H$6)-H37/H$6)+G37</f>
-        <v>1.6077922077922073</v>
-      </c>
-      <c r="G37">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H37">
-        <f t="shared" si="5"/>
-        <v>2.9000000000000012</v>
-      </c>
-      <c r="J37" s="10">
-        <f>A37-A38</f>
-        <v>5.8928571428571441E-2</v>
-      </c>
-      <c r="K37" s="10">
-        <f t="shared" si="1"/>
         <v>5.9090909090909083E-2</v>
       </c>
       <c r="N37">
-        <f>A37-F37</f>
+        <f t="shared" si="3"/>
         <v>5.1484795692112506E-2</v>
       </c>
       <c r="P37" s="6"/>
@@ -2753,30 +2751,30 @@
         <v>0.6</v>
       </c>
       <c r="C38">
+        <f t="shared" si="8"/>
+        <v>3.0000000000000013</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="1"/>
+        <v>1.5487012987012982</v>
+      </c>
+      <c r="G38">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="9"/>
+        <v>3.0000000000000013</v>
+      </c>
+      <c r="J38" s="10">
+        <f t="shared" si="2"/>
+        <v>5.8928571428571441E-2</v>
+      </c>
+      <c r="K38" s="10">
         <f t="shared" si="4"/>
-        <v>3.0000000000000013</v>
-      </c>
-      <c r="F38">
-        <f>F$6*(G38*(1/G$6+1/H$6)-H38/H$6)+G38</f>
-        <v>1.5487012987012982</v>
-      </c>
-      <c r="G38">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H38">
-        <f t="shared" si="5"/>
-        <v>3.0000000000000013</v>
-      </c>
-      <c r="J38" s="10">
-        <f>A38-A39</f>
-        <v>5.8928571428571441E-2</v>
-      </c>
-      <c r="K38" s="10">
-        <f t="shared" si="1"/>
         <v>5.9090909090909305E-2</v>
       </c>
       <c r="N38">
-        <f>A38-F38</f>
+        <f t="shared" si="3"/>
         <v>5.1647133354450148E-2</v>
       </c>
       <c r="P38" s="6"/>
@@ -2794,26 +2792,26 @@
         <v>3.1000000000000014</v>
       </c>
       <c r="F39">
-        <f>F$6*(G39*(1/G$6+1/H$6)-H39/H$6)+G39</f>
+        <f t="shared" si="1"/>
         <v>1.4896103896103889</v>
       </c>
       <c r="G39">
         <v>1.1000000000000001</v>
       </c>
       <c r="H39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3.1000000000000014</v>
       </c>
       <c r="J39" s="10">
-        <f>A39-A40</f>
+        <f t="shared" si="2"/>
         <v>5.8928571428571441E-2</v>
       </c>
       <c r="K39" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5.9090909090909305E-2</v>
       </c>
       <c r="N39">
-        <f>A39-F39</f>
+        <f t="shared" si="3"/>
         <v>5.1809471016788011E-2</v>
       </c>
       <c r="P39" s="6"/>
@@ -2827,30 +2825,30 @@
         <v>0.6</v>
       </c>
       <c r="C40">
-        <f t="shared" ref="C40:C41" si="6">C39+0.1</f>
+        <f t="shared" ref="C40:C41" si="10">C39+0.1</f>
         <v>3.2000000000000015</v>
       </c>
       <c r="F40">
-        <f>F$6*(G40*(1/G$6+1/H$6)-H40/H$6)+G40</f>
+        <f t="shared" si="1"/>
         <v>1.4305194805194796</v>
       </c>
       <c r="G40">
         <v>1.1000000000000001</v>
       </c>
       <c r="H40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3.2000000000000015</v>
       </c>
       <c r="J40" s="10">
-        <f>A40-A41</f>
+        <f t="shared" si="2"/>
         <v>5.8928571428571441E-2</v>
       </c>
       <c r="K40" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5.9090909090909083E-2</v>
       </c>
       <c r="N40">
-        <f>A40-F40</f>
+        <f t="shared" si="3"/>
         <v>5.1971808679125875E-2</v>
       </c>
       <c r="P40" s="6"/>
@@ -2864,23 +2862,23 @@
         <v>0.6</v>
       </c>
       <c r="C41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>3.3000000000000016</v>
       </c>
       <c r="F41">
-        <f>F$6*(G41*(1/G$6+1/H$6)-H41/H$6)+G41</f>
+        <f t="shared" si="1"/>
         <v>1.3714285714285706</v>
       </c>
       <c r="G41">
         <v>1.1000000000000001</v>
       </c>
       <c r="H41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3.3000000000000016</v>
       </c>
       <c r="J41" s="6"/>
       <c r="N41">
-        <f>A41-F41</f>
+        <f t="shared" si="3"/>
         <v>5.2134146341463516E-2</v>
       </c>
       <c r="P41" s="6"/>
@@ -2903,7 +2901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>

</xml_diff>